<commit_message>
fckeditor, an old one deleted
</commit_message>
<xml_diff>
--- a/files/listingfiles/OM Registration Sheet 2073.xlsx
+++ b/files/listingfiles/OM Registration Sheet 2073.xlsx
@@ -9,14 +9,16 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$2</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="239">
   <si>
     <t>k|fËfl/s dn cg'bfg -lhNnf:t/_ sfo{lalw @)&amp;@ cg';f/ rfn' cf=a= @)&amp;#÷&amp;$ sf] nflu ;"lrs[t k|fËfl/s dn pBf]ux?</t>
   </si>
@@ -131,6 +133,9 @@
   </si>
   <si>
     <t>lalqm kl/df0f d]=6g</t>
+  </si>
+  <si>
+    <t>k|f/De afof]6]s k|f=nL, /fdsf]6 sf7df08f}      a|f08M eld{sDkf]i6 !=%$M!=@@M!=%! gfMkmMkf]</t>
   </si>
   <si>
     <t>lalqm ug{ rfx]sf] kl/df0f d]=6g</t>
@@ -602,9 +607,6 @@
     <t>!=%@</t>
   </si>
   <si>
-    <t>!# lhNNf</t>
-  </si>
-  <si>
     <t>Kofn]6 d"No b/ ? k|lt s]hL 9'jfgL ;d]t</t>
   </si>
   <si>
@@ -618,13 +620,199 @@
   </si>
   <si>
     <t>bfg]bf/  ? #%, Kofn]6 ? #*</t>
+  </si>
+  <si>
+    <t>)&amp;#÷)&amp;÷!(</t>
+  </si>
+  <si>
+    <t>!@</t>
+  </si>
+  <si>
+    <t>e"dL k|fufl/s dn</t>
+  </si>
+  <si>
+    <t>#=@@</t>
+  </si>
+  <si>
+    <t>#=$$</t>
+  </si>
+  <si>
+    <t>!=%!</t>
+  </si>
+  <si>
+    <t>!# lhNNff</t>
+  </si>
+  <si>
+    <t>9'jfgL afx]s ? @#÷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pu|f]6]s dlN6g]zgn k|f=nL df8L—$ lrtjg e"dL k|f+ufl/s dn #=@@ M #=$$ M !=%! gfMkmMkf]M </t>
+  </si>
+  <si>
+    <t>Pu|f]6]s dlN6g]zgn k|f=nL df8L—$ lrtjg,  af;'b]j ;fksf]6f kmf]g g++ (*%%)%#)##</t>
+  </si>
+  <si>
+    <t>$^%)</t>
+  </si>
+  <si>
+    <t>!#</t>
+  </si>
+  <si>
+    <t>k|f/De afof]6]s k|f=nL, /fdsf]6 sf7df08f} ;Dks{ dlg; k|tfk (*%!!%(^#&amp;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">e"– </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Doc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> / e"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">– Doc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t>6«fO{sf]]8«df ;d]t</t>
+    </r>
+  </si>
+  <si>
+    <t>)=&amp;$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> !$ lhNnf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9'jfgL afx]s ? @#÷ / 6«fO{sf]]8«df o'Qm ? @% </t>
+  </si>
+  <si>
+    <t>6«fO{sf]]8«df ;d]td"No b/ ? k|lt s]hL 9'jfgL afx]s</t>
+  </si>
+  <si>
+    <t>eld{ d"No b/ ? k|lt s]hL 9'jfgL afx]s</t>
+  </si>
+  <si>
+    <t>^@)</t>
+  </si>
+  <si>
+    <t>!$</t>
+  </si>
+  <si>
+    <t>)&amp;#÷)&amp;÷@$</t>
+  </si>
+  <si>
+    <t>gy{lkmN8 k|fËfl/s dn sf/vfgf k|f=nL= 5]k]6f/ ;Dks{ an axfb'/ lwtfn kmf]g g++ (*$##)%@*@</t>
+  </si>
+  <si>
+    <t>gy{ lkmN8 k|fufl/s dn</t>
+  </si>
+  <si>
+    <t>!=&amp;@</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @=#$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $( lhNnf</t>
+  </si>
+  <si>
+    <t>gy{lkmN8 k|fËfl/s dn sf/vfgf k|f=nL= 5]k]6f/ a|f08M k|f= w'nf], !=&amp;@M @=@$ M!=%# gfMkmMkf]</t>
+  </si>
+  <si>
+    <t>ef*f afx]s 25</t>
+  </si>
+  <si>
+    <t>d"No b/ ? k|lt s]hL 9'jfgL ';d]t</t>
+  </si>
+  <si>
+    <t>!%</t>
+  </si>
+  <si>
+    <t>!^</t>
+  </si>
+  <si>
+    <t>g]zgn afof]6]s k|f=nL, n]n] nlntk'/, ;fyL bfg]bf/ tyf w'nf]dn !=%&amp;M!=^#M!=^@ gfMkmMkf]M</t>
+  </si>
+  <si>
+    <t>)&amp;#÷)*÷)^</t>
+  </si>
+  <si>
+    <t>;fyL bfg]bf/ tyf w'nf]dn</t>
+  </si>
+  <si>
+    <t>!=%&amp;</t>
+  </si>
+  <si>
+    <t>!=^#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!=^@ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> !# lhNnf</t>
+  </si>
+  <si>
+    <t>!%))</t>
+  </si>
+  <si>
+    <t>g]zgn afof]6]s k|f=nL, n]n] nlntk'/,  ;Dks{ Zofd ljqmd l;hfktL kmf]g (*%!!%)%)*, (*%!!%)%*%</t>
+  </si>
+  <si>
+    <t>w'nf] d"No b/ ? k|lt s]hL 9'jfgL ;d]t</t>
+  </si>
+  <si>
+    <t>bfgfbf/ d"No b/ ? k|lt s]hL 9'jfgL ;d]t</t>
+  </si>
+  <si>
+    <t>8An' 8An' Pu|f]6]s k|f=nL b]ar'nL –!$ k|utLgu/ gjnk/f;L, l6sf]k]Gb| zdf{ (*$%&amp;!@#&amp;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pj{/f e"–dn, w'nf] </t>
+  </si>
+  <si>
+    <t>8An' 8An' Pu|f]6]s k|f=nL= b]jr'nL–!$ k|ultgu/ gjnk/f;L, pj{/f e"–dn, w'nf] @ M @M @ M  gfMkmMkf]M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $# lhNnf</t>
+  </si>
+  <si>
+    <t>%%%)</t>
+  </si>
+  <si>
+    <t>9'jfgL afx]s ? @#.</t>
+  </si>
+  <si>
+    <t>)&amp;#÷)*÷!)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,6 +874,17 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Preeti"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Preeti"/>
     </font>
@@ -760,7 +959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -809,11 +1008,17 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -823,9 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1121,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1139,27 +1341,27 @@
     <col min="8" max="8" width="7.85546875" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="40.5" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-    </row>
-    <row r="2" spans="1:16" ht="54">
+      <c r="A1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" ht="36">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1191,7 +1393,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>16</v>
@@ -1212,7 +1414,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>12</v>
@@ -1227,7 +1429,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J3" s="14">
         <v>690</v>
@@ -1242,31 +1444,31 @@
     </row>
     <row r="4" spans="1:16" ht="72">
       <c r="A4" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -1274,31 +1476,31 @@
     </row>
     <row r="5" spans="1:16" ht="106.5" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="D5" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J5" s="14">
         <v>6857</v>
@@ -1308,31 +1510,31 @@
     </row>
     <row r="6" spans="1:16" ht="105.75" customHeight="1">
       <c r="A6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J6" s="14">
         <v>6815</v>
@@ -1342,31 +1544,31 @@
     </row>
     <row r="7" spans="1:16" ht="89.25" customHeight="1">
       <c r="A7" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>127</v>
-      </c>
       <c r="D7" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>133</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>132</v>
       </c>
       <c r="J7" s="14">
         <v>4265</v>
@@ -1376,31 +1578,31 @@
     </row>
     <row r="8" spans="1:16" ht="90">
       <c r="A8" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>135</v>
-      </c>
       <c r="D8" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J8" s="14">
         <v>1680</v>
@@ -1410,31 +1612,31 @@
     </row>
     <row r="9" spans="1:16" s="20" customFormat="1" ht="72">
       <c r="A9" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>143</v>
-      </c>
       <c r="I9" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J9" s="14">
         <v>4905</v>
@@ -1444,31 +1646,31 @@
     </row>
     <row r="10" spans="1:16" ht="72">
       <c r="A10" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>149</v>
-      </c>
       <c r="D10" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J10" s="14">
         <v>610</v>
@@ -1478,31 +1680,31 @@
     </row>
     <row r="11" spans="1:16" ht="90">
       <c r="A11" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>164</v>
       </c>
       <c r="J11" s="14">
         <v>880</v>
@@ -1512,31 +1714,31 @@
     </row>
     <row r="12" spans="1:16" ht="72">
       <c r="A12" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>167</v>
-      </c>
       <c r="D12" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>172</v>
-      </c>
       <c r="I12" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J12" s="22">
         <v>3005</v>
@@ -1546,31 +1748,31 @@
     </row>
     <row r="13" spans="1:16" ht="72">
       <c r="A13" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>176</v>
-      </c>
       <c r="D13" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E13" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>179</v>
-      </c>
       <c r="G13" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>187</v>
@@ -1579,6 +1781,180 @@
         <v>188</v>
       </c>
       <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" ht="72">
+      <c r="A14" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" ht="72">
+      <c r="A15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" ht="72">
+      <c r="A16" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="90">
+      <c r="A17" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="K17" s="18"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="72">
+      <c r="A18" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="L18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1589,170 +1965,218 @@
     <hyperlink ref="G12" r:id="rId2"/>
     <hyperlink ref="I12" r:id="rId3"/>
     <hyperlink ref="H13" r:id="rId4"/>
+    <hyperlink ref="C14" r:id="rId5"/>
+    <hyperlink ref="A14" r:id="rId6"/>
+    <hyperlink ref="A15" r:id="rId7" display="!@"/>
+    <hyperlink ref="C15" r:id="rId8" display="!@"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="J15" r:id="rId10"/>
+    <hyperlink ref="A16" r:id="rId11" display="!@"/>
+    <hyperlink ref="C16" r:id="rId12" display="!@"/>
+    <hyperlink ref="F16" r:id="rId13"/>
+    <hyperlink ref="A17" r:id="rId14" display="!@"/>
+    <hyperlink ref="C17" r:id="rId15" display="!@"/>
+    <hyperlink ref="C18" r:id="rId16" display="!@"/>
+    <hyperlink ref="A18" r:id="rId17" display="!@"/>
   </hyperlinks>
-  <pageMargins left="0.32" right="0.24" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="80" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageMargins left="0.32" right="0.24" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup scale="80" orientation="landscape" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X81"/>
+  <dimension ref="A1:AJ81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P5" sqref="P5"/>
+      <selection pane="topRight" activeCell="AM34" sqref="AM34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="11" customFormat="1" ht="22.5">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:36" s="11" customFormat="1" ht="22.5">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-    </row>
-    <row r="2" spans="1:24" ht="138" customHeight="1">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+    </row>
+    <row r="2" spans="1:36" ht="138" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="29" t="s">
+      <c r="B2" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29" t="s">
+      <c r="O2" s="27"/>
+      <c r="P2" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-    </row>
-    <row r="3" spans="1:24" ht="117">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ2" s="26"/>
+    </row>
+    <row r="3" spans="1:36" ht="114" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="E3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="I3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="M3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="O3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="Q3" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>36</v>
+        <v>218</v>
       </c>
       <c r="V3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="W3" s="9" t="s">
         <v>184</v>
@@ -1760,10 +2184,46 @@
       <c r="X3" s="9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="21">
+      <c r="Y3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="21">
       <c r="A4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1812,10 +2272,36 @@
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="23"/>
-    </row>
-    <row r="5" spans="1:24" ht="21">
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7">
+        <v>30</v>
+      </c>
+      <c r="AE4" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF4" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG4" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ4" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="21">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1844,10 +2330,32 @@
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="23"/>
-    </row>
-    <row r="6" spans="1:24" ht="21">
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="21">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1876,8 +2384,34 @@
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="23"/>
-    </row>
-    <row r="7" spans="1:24" ht="21">
+      <c r="Y6" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG6" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH6" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI6" s="7">
+        <v>150</v>
+      </c>
+      <c r="AJ6" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="21">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -1936,10 +2470,40 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="23"/>
-    </row>
-    <row r="8" spans="1:24" ht="21">
+      <c r="Y7" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z7" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE7" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF7" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH7" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI7" s="7">
+        <v>50</v>
+      </c>
+      <c r="AJ7" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="21">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1988,10 +2552,26 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="23"/>
-    </row>
-    <row r="9" spans="1:24" ht="21">
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" ht="21">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2036,10 +2616,30 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="23"/>
-    </row>
-    <row r="10" spans="1:24" ht="21">
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7">
+        <v>150</v>
+      </c>
+      <c r="AJ9" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="21">
       <c r="A10" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2092,10 +2692,30 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="23"/>
-    </row>
-    <row r="11" spans="1:24" ht="21">
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7">
+        <v>150</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ10" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="21">
       <c r="A11" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2124,8 +2744,30 @@
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="23"/>
-    </row>
-    <row r="12" spans="1:24" ht="21">
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7">
+        <v>25</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ11" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="21">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -2184,8 +2826,32 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="23"/>
-    </row>
-    <row r="13" spans="1:24" ht="21">
+      <c r="Y12" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7">
+        <v>200</v>
+      </c>
+      <c r="AE12" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ12" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="21">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -2244,10 +2910,34 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="23"/>
-    </row>
-    <row r="14" spans="1:24" ht="21">
+      <c r="Y13" s="7">
+        <v>400</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7">
+        <v>500</v>
+      </c>
+      <c r="AE13" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ13" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="21">
       <c r="A14" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2292,10 +2982,30 @@
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="23"/>
-    </row>
-    <row r="15" spans="1:24" ht="21">
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7">
+        <v>40</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>55</v>
+      </c>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ14" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="21">
       <c r="A15" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2332,10 +3042,32 @@
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="23"/>
-    </row>
-    <row r="16" spans="1:24" ht="21">
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7">
+        <v>30</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>30</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>55</v>
+      </c>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+    </row>
+    <row r="16" spans="1:36" ht="21">
       <c r="A16" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2380,10 +3112,30 @@
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="23"/>
-    </row>
-    <row r="17" spans="1:24" ht="21">
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE16" s="7">
+        <v>55</v>
+      </c>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ16" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="21">
       <c r="A17" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2436,8 +3188,28 @@
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="23"/>
-    </row>
-    <row r="18" spans="1:24" ht="21">
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE17" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ17" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="21">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
@@ -2496,10 +3268,36 @@
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="23"/>
-    </row>
-    <row r="19" spans="1:24" ht="21">
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7">
+        <v>25</v>
+      </c>
+      <c r="AB18" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD18" s="7">
+        <v>125</v>
+      </c>
+      <c r="AE18" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ18" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="21">
       <c r="A19" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5">
         <v>50</v>
@@ -2556,10 +3354,26 @@
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="23"/>
-    </row>
-    <row r="20" spans="1:24" ht="21">
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7">
+        <v>300</v>
+      </c>
+      <c r="AE19" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+    </row>
+    <row r="20" spans="1:36" ht="21">
       <c r="A20" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2608,10 +3422,34 @@
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="23"/>
-    </row>
-    <row r="21" spans="1:24" ht="21">
+      <c r="Y20" s="7">
+        <v>400</v>
+      </c>
+      <c r="Z20" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7">
+        <v>500</v>
+      </c>
+      <c r="AE20" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7">
+        <v>250</v>
+      </c>
+      <c r="AJ20" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="21">
       <c r="A21" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2656,8 +3494,32 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="23"/>
-    </row>
-    <row r="22" spans="1:24" ht="21">
+      <c r="Y21" s="7">
+        <v>50</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE21" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ21" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" ht="21">
       <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
@@ -2712,8 +3574,38 @@
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="23"/>
-    </row>
-    <row r="23" spans="1:24" ht="21">
+      <c r="Y22" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z22" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>50</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC22" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD22" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE22" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ22" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="21">
       <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
@@ -2768,8 +3660,28 @@
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="23"/>
-    </row>
-    <row r="24" spans="1:24" ht="21">
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7">
+        <v>250</v>
+      </c>
+      <c r="AE23" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ23" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="21">
       <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
@@ -2828,10 +3740,34 @@
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="23"/>
-    </row>
-    <row r="25" spans="1:24" ht="21">
+      <c r="Y24" s="7">
+        <v>350</v>
+      </c>
+      <c r="Z24" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7">
+        <v>200</v>
+      </c>
+      <c r="AE24" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ24" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="21">
       <c r="A25" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2864,10 +3800,30 @@
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="23"/>
-    </row>
-    <row r="26" spans="1:24" ht="21">
+      <c r="Y25" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ25" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="21">
       <c r="A26" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2896,10 +3852,38 @@
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="23"/>
-    </row>
-    <row r="27" spans="1:24" ht="21">
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC26" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD26" s="7"/>
+      <c r="AE26" s="7"/>
+      <c r="AF26" s="7">
+        <v>50</v>
+      </c>
+      <c r="AG26" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH26" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI26" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ26" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="21">
       <c r="A27" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2954,10 +3938,42 @@
       <c r="X27" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" ht="21">
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7">
+        <v>25</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD27" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE27" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG27" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH27" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI27" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ27" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="21">
       <c r="A28" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2992,10 +4008,38 @@
       <c r="X28" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" ht="21">
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7">
+        <v>15</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD28" s="7"/>
+      <c r="AE28" s="7"/>
+      <c r="AF28" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG28" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH28" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI28" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ28" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="21">
       <c r="A29" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3040,8 +4084,40 @@
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
-    </row>
-    <row r="30" spans="1:24" ht="21">
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD29" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE29" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF29" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG29" s="7">
+        <v>26</v>
+      </c>
+      <c r="AH29" s="7">
+        <v>38</v>
+      </c>
+      <c r="AI29" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ29" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="21">
       <c r="A30" s="8" t="s">
         <v>27</v>
       </c>
@@ -3104,8 +4180,44 @@
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
-    </row>
-    <row r="31" spans="1:24" ht="21">
+      <c r="Y30" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z30" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA30" s="7">
+        <v>25</v>
+      </c>
+      <c r="AB30" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC30" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD30" s="7">
+        <v>300</v>
+      </c>
+      <c r="AE30" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF30" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG30" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH30" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI30" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ30" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="21">
       <c r="A31" s="8" t="s">
         <v>25</v>
       </c>
@@ -3170,8 +4282,40 @@
       <c r="X31" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" ht="21">
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7">
+        <v>300</v>
+      </c>
+      <c r="AB31" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC31" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD31" s="7">
+        <v>1000</v>
+      </c>
+      <c r="AE31" s="7">
+        <v>27</v>
+      </c>
+      <c r="AF31" s="7">
+        <v>200</v>
+      </c>
+      <c r="AG31" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH31" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI31" s="7">
+        <v>400</v>
+      </c>
+      <c r="AJ31" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="21">
       <c r="A32" s="8" t="s">
         <v>26</v>
       </c>
@@ -3236,10 +4380,42 @@
       <c r="X32" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" ht="21">
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7">
+        <v>50</v>
+      </c>
+      <c r="AB32" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC32" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD32" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE32" s="7">
+        <v>27</v>
+      </c>
+      <c r="AF32" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG32" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH32" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI32" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ32" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="21">
       <c r="A33" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3274,10 +4450,38 @@
       <c r="X33" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" ht="21">
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7">
+        <v>25</v>
+      </c>
+      <c r="AB33" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC33" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7">
+        <v>250</v>
+      </c>
+      <c r="AG33" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH33" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI33" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ33" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="21">
       <c r="A34" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3332,8 +4536,38 @@
       <c r="X34" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" ht="21">
+      <c r="Y34" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z34" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE34" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF34" s="7">
+        <v>100</v>
+      </c>
+      <c r="AG34" s="7">
+        <v>30</v>
+      </c>
+      <c r="AH34" s="7">
+        <v>42</v>
+      </c>
+      <c r="AI34" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ34" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" ht="21">
       <c r="A35" s="8" t="s">
         <v>24</v>
       </c>
@@ -3402,10 +4636,40 @@
       <c r="X35" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" ht="21">
+      <c r="Y35" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z35" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA35" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB35" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC35" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD35" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE35" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ35" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="21">
       <c r="A36" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3434,10 +4698,30 @@
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
-    </row>
-    <row r="37" spans="1:24" ht="21">
+      <c r="Y36" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7">
+        <v>50</v>
+      </c>
+      <c r="AJ36" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" ht="21">
       <c r="A37" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3466,10 +4750,30 @@
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
-    </row>
-    <row r="38" spans="1:24" ht="21">
+      <c r="Y37" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z37" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ37" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="21">
       <c r="A38" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3498,10 +4802,26 @@
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
-    </row>
-    <row r="39" spans="1:24" ht="21">
+      <c r="Y38" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z38" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+    </row>
+    <row r="39" spans="1:36" ht="21">
       <c r="A39" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3552,10 +4872,26 @@
       <c r="X39" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" ht="21">
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7">
+        <v>150</v>
+      </c>
+      <c r="AE39" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+    </row>
+    <row r="40" spans="1:36" ht="21">
       <c r="A40" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3590,10 +4926,22 @@
       <c r="X40" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" ht="21">
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="7"/>
+      <c r="AB40" s="7"/>
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7"/>
+      <c r="AE40" s="7"/>
+      <c r="AF40" s="7"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
+      <c r="AJ40" s="7"/>
+    </row>
+    <row r="41" spans="1:36" ht="21">
       <c r="A41" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3618,10 +4966,22 @@
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
-    </row>
-    <row r="42" spans="1:24" ht="21">
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7"/>
+      <c r="AC41" s="7"/>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+    </row>
+    <row r="42" spans="1:36" ht="51.75">
       <c r="A42" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -3676,8 +5036,28 @@
       <c r="X42" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" ht="21">
+      <c r="Y42" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z42" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA42" s="7"/>
+      <c r="AB42" s="7"/>
+      <c r="AC42" s="7"/>
+      <c r="AD42" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE42" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="AF42" s="7"/>
+      <c r="AG42" s="7"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="7"/>
+      <c r="AJ42" s="7"/>
+    </row>
+    <row r="43" spans="1:36" ht="21">
       <c r="A43" s="8" t="s">
         <v>28</v>
       </c>
@@ -3742,10 +5122,34 @@
       <c r="X43" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" ht="21">
+      <c r="Y43" s="7">
+        <v>200</v>
+      </c>
+      <c r="Z43" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7"/>
+      <c r="AC43" s="7"/>
+      <c r="AD43" s="7">
+        <v>300</v>
+      </c>
+      <c r="AE43" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ43" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" ht="21">
       <c r="A44" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -3794,10 +5198,34 @@
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
-    </row>
-    <row r="45" spans="1:24" ht="21">
+      <c r="Y44" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z44" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="7"/>
+      <c r="AC44" s="7"/>
+      <c r="AD44" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE44" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ44" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" ht="21">
       <c r="A45" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -3850,10 +5278,30 @@
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
-    </row>
-    <row r="46" spans="1:24" ht="21">
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="7"/>
+      <c r="AD45" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE45" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ45" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" ht="21">
       <c r="A46" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -3886,10 +5334,22 @@
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
-    </row>
-    <row r="47" spans="1:24" ht="21">
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="7"/>
+      <c r="AB46" s="7"/>
+      <c r="AC46" s="7"/>
+      <c r="AD46" s="7"/>
+      <c r="AE46" s="7"/>
+      <c r="AF46" s="7"/>
+      <c r="AG46" s="7"/>
+      <c r="AH46" s="7"/>
+      <c r="AI46" s="7"/>
+      <c r="AJ46" s="7"/>
+    </row>
+    <row r="47" spans="1:36" ht="21">
       <c r="A47" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -3930,10 +5390,26 @@
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
-    </row>
-    <row r="48" spans="1:24" ht="21">
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
+      <c r="AC47" s="7"/>
+      <c r="AD47" s="7">
+        <v>20</v>
+      </c>
+      <c r="AE47" s="7">
+        <v>50</v>
+      </c>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7"/>
+    </row>
+    <row r="48" spans="1:36" ht="21">
       <c r="A48" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -3972,10 +5448,26 @@
       <c r="X48" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" ht="21">
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="7"/>
+      <c r="AB48" s="7"/>
+      <c r="AC48" s="7"/>
+      <c r="AD48" s="7"/>
+      <c r="AE48" s="7"/>
+      <c r="AF48" s="7"/>
+      <c r="AG48" s="7"/>
+      <c r="AH48" s="7"/>
+      <c r="AI48" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ48" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" ht="21">
       <c r="A49" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -4008,10 +5500,22 @@
       <c r="V49" s="5"/>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
-    </row>
-    <row r="50" spans="1:24" ht="21">
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7"/>
+      <c r="AC49" s="7"/>
+      <c r="AD49" s="7"/>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+    </row>
+    <row r="50" spans="1:36" ht="21">
       <c r="A50" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -4056,10 +5560,26 @@
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
-    </row>
-    <row r="51" spans="1:24" ht="21">
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="7">
+        <v>20</v>
+      </c>
+      <c r="AE50" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF50" s="7"/>
+      <c r="AG50" s="7"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7"/>
+    </row>
+    <row r="51" spans="1:36" ht="21">
       <c r="A51" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -4112,8 +5632,28 @@
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
-    </row>
-    <row r="52" spans="1:24" ht="21">
+      <c r="Y51" s="7">
+        <v>50</v>
+      </c>
+      <c r="Z51" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="7">
+        <v>40</v>
+      </c>
+      <c r="AE51" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+    </row>
+    <row r="52" spans="1:36" ht="21">
       <c r="A52" s="8" t="s">
         <v>29</v>
       </c>
@@ -4178,10 +5718,40 @@
       <c r="X52" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" ht="21">
+      <c r="Y52" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z52" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA52" s="7">
+        <v>20</v>
+      </c>
+      <c r="AB52" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC52" s="7">
+        <v>25</v>
+      </c>
+      <c r="AD52" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE52" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF52" s="7"/>
+      <c r="AG52" s="7"/>
+      <c r="AH52" s="7"/>
+      <c r="AI52" s="7">
+        <v>200</v>
+      </c>
+      <c r="AJ52" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" ht="21">
       <c r="A53" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -4230,8 +5800,32 @@
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
       <c r="X53" s="5"/>
-    </row>
-    <row r="54" spans="1:24" ht="21">
+      <c r="Y53" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7"/>
+      <c r="AC53" s="7"/>
+      <c r="AD53" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE53" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ53" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" ht="21">
       <c r="A54" s="8" t="s">
         <v>30</v>
       </c>
@@ -4286,10 +5880,30 @@
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
       <c r="X54" s="5"/>
-    </row>
-    <row r="55" spans="1:24" ht="21">
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+      <c r="AC54" s="7"/>
+      <c r="AD54" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE54" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF54" s="7"/>
+      <c r="AG54" s="7"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ54" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" ht="21">
       <c r="A55" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -4330,10 +5944,26 @@
       <c r="V55" s="5"/>
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
-    </row>
-    <row r="56" spans="1:24" ht="21">
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7"/>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7"/>
+      <c r="AC55" s="7"/>
+      <c r="AD55" s="7">
+        <v>20</v>
+      </c>
+      <c r="AE55" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+    </row>
+    <row r="56" spans="1:36" ht="21">
       <c r="A56" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -4366,10 +5996,22 @@
       <c r="V56" s="5"/>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
-    </row>
-    <row r="57" spans="1:24" ht="21">
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
+      <c r="AC56" s="7"/>
+      <c r="AD56" s="7"/>
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="7"/>
+      <c r="AG56" s="7"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="7"/>
+      <c r="AJ56" s="7"/>
+    </row>
+    <row r="57" spans="1:36" ht="21">
       <c r="A57" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -4398,10 +6040,22 @@
       <c r="V57" s="5"/>
       <c r="W57" s="5"/>
       <c r="X57" s="5"/>
-    </row>
-    <row r="58" spans="1:24" ht="21">
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7"/>
+      <c r="AC57" s="7"/>
+      <c r="AD57" s="7"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+    </row>
+    <row r="58" spans="1:36" ht="21">
       <c r="A58" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -4442,10 +6096,26 @@
       <c r="V58" s="5"/>
       <c r="W58" s="5"/>
       <c r="X58" s="5"/>
-    </row>
-    <row r="59" spans="1:24" ht="21">
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="7"/>
+      <c r="AB58" s="7"/>
+      <c r="AC58" s="7"/>
+      <c r="AD58" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE58" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF58" s="7"/>
+      <c r="AG58" s="7"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="7"/>
+      <c r="AJ58" s="7"/>
+    </row>
+    <row r="59" spans="1:36" ht="21">
       <c r="A59" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B59" s="5">
         <v>25</v>
@@ -4494,10 +6164,34 @@
       <c r="V59" s="5"/>
       <c r="W59" s="5"/>
       <c r="X59" s="5"/>
-    </row>
-    <row r="60" spans="1:24" ht="21">
+      <c r="Y59" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z59" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7"/>
+      <c r="AC59" s="7"/>
+      <c r="AD59" s="7">
+        <v>200</v>
+      </c>
+      <c r="AE59" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ59" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" ht="21">
       <c r="A60" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -4542,10 +6236,26 @@
       <c r="V60" s="5"/>
       <c r="W60" s="5"/>
       <c r="X60" s="5"/>
-    </row>
-    <row r="61" spans="1:24" ht="21">
+      <c r="Y60" s="7"/>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="7"/>
+      <c r="AB60" s="7"/>
+      <c r="AC60" s="7"/>
+      <c r="AD60" s="7">
+        <v>300</v>
+      </c>
+      <c r="AE60" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF60" s="7"/>
+      <c r="AG60" s="7"/>
+      <c r="AH60" s="7"/>
+      <c r="AI60" s="7"/>
+      <c r="AJ60" s="7"/>
+    </row>
+    <row r="61" spans="1:36" ht="21">
       <c r="A61" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -4574,10 +6284,22 @@
       <c r="V61" s="5"/>
       <c r="W61" s="5"/>
       <c r="X61" s="5"/>
-    </row>
-    <row r="62" spans="1:24" ht="21">
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7"/>
+      <c r="AC61" s="7"/>
+      <c r="AD61" s="7"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7"/>
+    </row>
+    <row r="62" spans="1:36" ht="21">
       <c r="A62" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -4626,10 +6348,26 @@
       <c r="V62" s="5"/>
       <c r="W62" s="5"/>
       <c r="X62" s="5"/>
-    </row>
-    <row r="63" spans="1:24" ht="21">
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="7"/>
+      <c r="AB62" s="7"/>
+      <c r="AC62" s="7"/>
+      <c r="AD62" s="7">
+        <v>150</v>
+      </c>
+      <c r="AE62" s="7">
+        <v>35</v>
+      </c>
+      <c r="AF62" s="7"/>
+      <c r="AG62" s="7"/>
+      <c r="AH62" s="7"/>
+      <c r="AI62" s="7"/>
+      <c r="AJ62" s="7"/>
+    </row>
+    <row r="63" spans="1:36" ht="21">
       <c r="A63" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -4674,10 +6412,34 @@
       <c r="V63" s="5"/>
       <c r="W63" s="5"/>
       <c r="X63" s="5"/>
-    </row>
-    <row r="64" spans="1:24" ht="21">
+      <c r="Y63" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z63" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7"/>
+      <c r="AC63" s="7"/>
+      <c r="AD63" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE63" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ63" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" ht="21">
       <c r="A64" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -4706,10 +6468,30 @@
       <c r="V64" s="5"/>
       <c r="W64" s="5"/>
       <c r="X64" s="5"/>
-    </row>
-    <row r="65" spans="1:24" ht="21">
+      <c r="Y64" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z64" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA64" s="7"/>
+      <c r="AB64" s="7"/>
+      <c r="AC64" s="7"/>
+      <c r="AD64" s="7"/>
+      <c r="AE64" s="7"/>
+      <c r="AF64" s="7"/>
+      <c r="AG64" s="7"/>
+      <c r="AH64" s="7"/>
+      <c r="AI64" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ64" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" ht="21">
       <c r="A65" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -4762,10 +6544,26 @@
       <c r="V65" s="5"/>
       <c r="W65" s="5"/>
       <c r="X65" s="5"/>
-    </row>
-    <row r="66" spans="1:24" ht="21">
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
+      <c r="AC65" s="7"/>
+      <c r="AD65" s="7">
+        <v>200</v>
+      </c>
+      <c r="AE65" s="7">
+        <v>50</v>
+      </c>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+    </row>
+    <row r="66" spans="1:36" ht="21">
       <c r="A66" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -4794,10 +6592,22 @@
       <c r="V66" s="5"/>
       <c r="W66" s="5"/>
       <c r="X66" s="5"/>
-    </row>
-    <row r="67" spans="1:24" ht="21">
+      <c r="Y66" s="7"/>
+      <c r="Z66" s="7"/>
+      <c r="AA66" s="7"/>
+      <c r="AB66" s="7"/>
+      <c r="AC66" s="7"/>
+      <c r="AD66" s="7"/>
+      <c r="AE66" s="7"/>
+      <c r="AF66" s="7"/>
+      <c r="AG66" s="7"/>
+      <c r="AH66" s="7"/>
+      <c r="AI66" s="7"/>
+      <c r="AJ66" s="7"/>
+    </row>
+    <row r="67" spans="1:36" ht="21">
       <c r="A67" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -4826,10 +6636,22 @@
       <c r="V67" s="5"/>
       <c r="W67" s="5"/>
       <c r="X67" s="5"/>
-    </row>
-    <row r="68" spans="1:24" ht="21">
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7"/>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7"/>
+      <c r="AC67" s="7"/>
+      <c r="AD67" s="7"/>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+    </row>
+    <row r="68" spans="1:36" ht="21">
       <c r="A68" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -4858,10 +6680,22 @@
       <c r="V68" s="5"/>
       <c r="W68" s="5"/>
       <c r="X68" s="5"/>
-    </row>
-    <row r="69" spans="1:24" ht="21">
+      <c r="Y68" s="7"/>
+      <c r="Z68" s="7"/>
+      <c r="AA68" s="7"/>
+      <c r="AB68" s="7"/>
+      <c r="AC68" s="7"/>
+      <c r="AD68" s="7"/>
+      <c r="AE68" s="7"/>
+      <c r="AF68" s="7"/>
+      <c r="AG68" s="7"/>
+      <c r="AH68" s="7"/>
+      <c r="AI68" s="7"/>
+      <c r="AJ68" s="7"/>
+    </row>
+    <row r="69" spans="1:36" ht="21">
       <c r="A69" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -4890,10 +6724,22 @@
       <c r="V69" s="5"/>
       <c r="W69" s="5"/>
       <c r="X69" s="5"/>
-    </row>
-    <row r="70" spans="1:24" ht="21">
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7"/>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7"/>
+      <c r="AC69" s="7"/>
+      <c r="AD69" s="7"/>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7"/>
+    </row>
+    <row r="70" spans="1:36" ht="21">
       <c r="A70" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -4930,10 +6776,26 @@
       <c r="V70" s="5"/>
       <c r="W70" s="5"/>
       <c r="X70" s="5"/>
-    </row>
-    <row r="71" spans="1:24" ht="21">
+      <c r="Y70" s="7"/>
+      <c r="Z70" s="7"/>
+      <c r="AA70" s="7"/>
+      <c r="AB70" s="7"/>
+      <c r="AC70" s="7"/>
+      <c r="AD70" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE70" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF70" s="7"/>
+      <c r="AG70" s="7"/>
+      <c r="AH70" s="7"/>
+      <c r="AI70" s="7"/>
+      <c r="AJ70" s="7"/>
+    </row>
+    <row r="71" spans="1:36" ht="21">
       <c r="A71" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -4970,10 +6832,26 @@
       <c r="V71" s="5"/>
       <c r="W71" s="5"/>
       <c r="X71" s="5"/>
-    </row>
-    <row r="72" spans="1:24" ht="21">
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7"/>
+      <c r="AC71" s="7"/>
+      <c r="AD71" s="7">
+        <v>20</v>
+      </c>
+      <c r="AE71" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+    </row>
+    <row r="72" spans="1:36" ht="21">
       <c r="A72" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -5002,10 +6880,22 @@
       <c r="V72" s="5"/>
       <c r="W72" s="5"/>
       <c r="X72" s="5"/>
-    </row>
-    <row r="73" spans="1:24" ht="21">
+      <c r="Y72" s="7"/>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="7"/>
+      <c r="AB72" s="7"/>
+      <c r="AC72" s="7"/>
+      <c r="AD72" s="7"/>
+      <c r="AE72" s="7"/>
+      <c r="AF72" s="7"/>
+      <c r="AG72" s="7"/>
+      <c r="AH72" s="7"/>
+      <c r="AI72" s="7"/>
+      <c r="AJ72" s="7"/>
+    </row>
+    <row r="73" spans="1:36" ht="21">
       <c r="A73" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -5042,10 +6932,26 @@
       <c r="V73" s="5"/>
       <c r="W73" s="5"/>
       <c r="X73" s="23"/>
-    </row>
-    <row r="74" spans="1:24" ht="21">
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="7"/>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7"/>
+      <c r="AC73" s="7"/>
+      <c r="AD73" s="7">
+        <v>50</v>
+      </c>
+      <c r="AE73" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF73" s="7"/>
+      <c r="AG73" s="7"/>
+      <c r="AH73" s="7"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="7"/>
+    </row>
+    <row r="74" spans="1:36" ht="21">
       <c r="A74" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -5090,10 +6996,32 @@
       <c r="V74" s="5"/>
       <c r="W74" s="5"/>
       <c r="X74" s="23"/>
-    </row>
-    <row r="75" spans="1:24" ht="21">
+      <c r="Y74" s="7">
+        <v>300</v>
+      </c>
+      <c r="Z74" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA74" s="7"/>
+      <c r="AB74" s="7"/>
+      <c r="AC74" s="7"/>
+      <c r="AD74" s="7">
+        <v>200</v>
+      </c>
+      <c r="AE74" s="7">
+        <v>30</v>
+      </c>
+      <c r="AF74" s="7"/>
+      <c r="AG74" s="7"/>
+      <c r="AH74" s="7"/>
+      <c r="AI74" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ74" s="7"/>
+    </row>
+    <row r="75" spans="1:36" ht="21">
       <c r="A75" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -5122,10 +7050,26 @@
       <c r="V75" s="5"/>
       <c r="W75" s="5"/>
       <c r="X75" s="23"/>
-    </row>
-    <row r="76" spans="1:24" ht="21">
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7"/>
+      <c r="AC75" s="7"/>
+      <c r="AD75" s="7">
+        <v>30</v>
+      </c>
+      <c r="AE75" s="7">
+        <v>55</v>
+      </c>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7"/>
+    </row>
+    <row r="76" spans="1:36" ht="21">
       <c r="A76" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -5154,10 +7098,22 @@
       <c r="V76" s="5"/>
       <c r="W76" s="5"/>
       <c r="X76" s="23"/>
-    </row>
-    <row r="77" spans="1:24" ht="21">
+      <c r="Y76" s="7"/>
+      <c r="Z76" s="7"/>
+      <c r="AA76" s="7"/>
+      <c r="AB76" s="7"/>
+      <c r="AC76" s="7"/>
+      <c r="AD76" s="7"/>
+      <c r="AE76" s="7"/>
+      <c r="AF76" s="7"/>
+      <c r="AG76" s="7"/>
+      <c r="AH76" s="7"/>
+      <c r="AI76" s="7"/>
+      <c r="AJ76" s="7"/>
+    </row>
+    <row r="77" spans="1:36" ht="21">
       <c r="A77" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -5194,10 +7150,26 @@
       <c r="V77" s="5"/>
       <c r="W77" s="5"/>
       <c r="X77" s="23"/>
-    </row>
-    <row r="78" spans="1:24" ht="21">
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7"/>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7"/>
+      <c r="AC77" s="7"/>
+      <c r="AD77" s="7">
+        <v>100</v>
+      </c>
+      <c r="AE77" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+    </row>
+    <row r="78" spans="1:36" ht="21">
       <c r="A78" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -5228,8 +7200,26 @@
       <c r="V78" s="5"/>
       <c r="W78" s="5"/>
       <c r="X78" s="23"/>
-    </row>
-    <row r="79" spans="1:24" ht="17.25">
+      <c r="Y78" s="7">
+        <v>100</v>
+      </c>
+      <c r="Z78" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA78" s="7"/>
+      <c r="AB78" s="7"/>
+      <c r="AC78" s="7"/>
+      <c r="AD78" s="7"/>
+      <c r="AE78" s="7"/>
+      <c r="AF78" s="7"/>
+      <c r="AG78" s="7"/>
+      <c r="AH78" s="7"/>
+      <c r="AI78" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ78" s="7"/>
+    </row>
+    <row r="79" spans="1:36" ht="17.25">
       <c r="A79" s="10"/>
       <c r="B79" s="5">
         <f>SUM(B4:B78)</f>
@@ -5247,7 +7237,7 @@
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5">
-        <f t="shared" ref="H79:V79" si="1">SUM(H4:H78)</f>
+        <f t="shared" ref="H79:AI79" si="1">SUM(H4:H78)</f>
         <v>6815</v>
       </c>
       <c r="I79" s="5"/>
@@ -5287,8 +7277,35 @@
       </c>
       <c r="W79" s="5"/>
       <c r="X79" s="5"/>
-    </row>
-    <row r="80" spans="1:24">
+      <c r="Y79" s="5">
+        <f t="shared" si="1"/>
+        <v>4650</v>
+      </c>
+      <c r="Z79" s="5"/>
+      <c r="AA79" s="5">
+        <f t="shared" si="1"/>
+        <v>620</v>
+      </c>
+      <c r="AB79" s="5"/>
+      <c r="AC79" s="5"/>
+      <c r="AD79" s="5">
+        <f t="shared" si="1"/>
+        <v>7025</v>
+      </c>
+      <c r="AE79" s="5"/>
+      <c r="AF79" s="5">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="AG79" s="5"/>
+      <c r="AH79" s="5"/>
+      <c r="AI79" s="5">
+        <f t="shared" si="1"/>
+        <v>5550</v>
+      </c>
+      <c r="AJ79" s="5"/>
+    </row>
+    <row r="80" spans="1:36">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5303,12 +7320,8 @@
       <c r="E81" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="A1:X1"/>
+  <mergeCells count="17">
+    <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="R2:S2"/>
@@ -5316,20 +7329,17 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>